<commit_message>
Made basic data sheets for now. Can be improved easily later by editing script.
</commit_message>
<xml_diff>
--- a/docs/source/docs/ATP/procedures.xlsx
+++ b/docs/source/docs/ATP/procedures.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1E93C9E-3C8F-42B2-A95C-8C6CDD27932E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A646E3E9-0681-44FC-A9EE-C10815A267A2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="47880" yWindow="-120" windowWidth="29040" windowHeight="15225" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="2" r:id="rId1"/>
@@ -402,12 +402,6 @@
     <t>Target GUI Behavior Mapper Acceptance Test</t>
   </si>
   <si>
-    <t>This acceptance test document verifies that the software system, Facile has a GUI that contains a view that allows the users to specify ‘Show/Hide’ for relation between two components.  This acceptance test establishes the framework used by the acceptance test team to plan, execute, and document acceptance testing.  It describes the scope of the work performed and the approach taken to execute the tests created to validate that the system performs as required in the GUI. The details of this acceptance test are developed according to the requirements specifications and show traceability back to those specifications.</t>
-  </si>
-  <si>
-    <t>To verify SSR 4.3.1.2 The Facile GUI shall contain a view that allows user to specify ‘Show/Hide’ relation between two components.</t>
-  </si>
-  <si>
     <t>Click on the same button that you clicked on in the previous step.</t>
   </si>
   <si>
@@ -610,6 +604,12 @@
   </si>
   <si>
     <t>Verify that the *Python 3.7.4* and *32-bit* exist in the resulting text from the previous step.</t>
+  </si>
+  <si>
+    <t>To verify SSR 4.3.1.2 The Facile GUI shall contain a view that allows user to specify 'Show/Hide' relation between two components.</t>
+  </si>
+  <si>
+    <t>This acceptance test document verifies that the software system, Facile has a GUI that contains a view that allows the users to specify 'Show/Hide' for relation between two components.  This acceptance test establishes the framework used by the acceptance test team to plan, execute, and document acceptance testing.  It describes the scope of the work performed and the approach taken to execute the tests created to validate that the system performs as required in the GUI. The details of this acceptance test are developed according to the requirements specifications and show traceability back to those specifications.</t>
   </si>
 </sst>
 </file>
@@ -939,64 +939,127 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1025,17 +1088,14 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1045,66 +1105,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1388,8 +1388,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FAD1217-8B4A-4FAD-B4A9-6A7FF2C87FBC}">
   <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="K58" sqref="K58"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1400,828 +1400,846 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.3" x14ac:dyDescent="0.7">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="31"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="52"/>
     </row>
     <row r="2" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="34"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="55"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="32"/>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="34"/>
+      <c r="A3" s="53"/>
+      <c r="B3" s="54"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="54"/>
+      <c r="I3" s="55"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="32"/>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="34"/>
+      <c r="A4" s="53"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="54"/>
+      <c r="G4" s="54"/>
+      <c r="H4" s="54"/>
+      <c r="I4" s="55"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="32"/>
-      <c r="B5" s="33"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="34"/>
+      <c r="A5" s="53"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="54"/>
+      <c r="G5" s="54"/>
+      <c r="H5" s="54"/>
+      <c r="I5" s="55"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="32"/>
-      <c r="B6" s="33"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="34"/>
+      <c r="A6" s="53"/>
+      <c r="B6" s="54"/>
+      <c r="C6" s="54"/>
+      <c r="D6" s="54"/>
+      <c r="E6" s="54"/>
+      <c r="F6" s="54"/>
+      <c r="G6" s="54"/>
+      <c r="H6" s="54"/>
+      <c r="I6" s="55"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="32"/>
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="34"/>
+      <c r="A7" s="53"/>
+      <c r="B7" s="54"/>
+      <c r="C7" s="54"/>
+      <c r="D7" s="54"/>
+      <c r="E7" s="54"/>
+      <c r="F7" s="54"/>
+      <c r="G7" s="54"/>
+      <c r="H7" s="54"/>
+      <c r="I7" s="55"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="32"/>
-      <c r="B8" s="33"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="33"/>
-      <c r="I8" s="34"/>
+      <c r="A8" s="53"/>
+      <c r="B8" s="54"/>
+      <c r="C8" s="54"/>
+      <c r="D8" s="54"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="54"/>
+      <c r="G8" s="54"/>
+      <c r="H8" s="54"/>
+      <c r="I8" s="55"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="32"/>
-      <c r="B9" s="33"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="34"/>
+      <c r="A9" s="53"/>
+      <c r="B9" s="54"/>
+      <c r="C9" s="54"/>
+      <c r="D9" s="54"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="54"/>
+      <c r="G9" s="54"/>
+      <c r="H9" s="54"/>
+      <c r="I9" s="55"/>
     </row>
     <row r="10" spans="1:9" ht="18.3" x14ac:dyDescent="0.7">
-      <c r="A10" s="35" t="s">
+      <c r="A10" s="56" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="36"/>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="37"/>
+      <c r="B10" s="57"/>
+      <c r="C10" s="57"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="57"/>
+      <c r="H10" s="57"/>
+      <c r="I10" s="58"/>
     </row>
     <row r="11" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="38"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="25"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="20"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="38"/>
+      <c r="A12" s="23"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="25"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="20"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="38"/>
+      <c r="A13" s="23"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="25"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="20"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="38"/>
+      <c r="A14" s="23"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="25"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="20"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="38"/>
+      <c r="A15" s="23"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="25"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="20"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="38"/>
+      <c r="A16" s="23"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="25"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="20"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="38"/>
+      <c r="A17" s="23"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="25"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="20"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="38"/>
+      <c r="A18" s="23"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="25"/>
     </row>
     <row r="19" spans="1:9" ht="16.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="42">
+      <c r="A19" s="62">
         <v>1</v>
       </c>
-      <c r="B19" s="62" t="s">
+      <c r="B19" s="59" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="63"/>
-      <c r="D19" s="63"/>
-      <c r="E19" s="63"/>
-      <c r="F19" s="63"/>
-      <c r="G19" s="63"/>
-      <c r="H19" s="63"/>
-      <c r="I19" s="64"/>
+      <c r="C19" s="60"/>
+      <c r="D19" s="60"/>
+      <c r="E19" s="60"/>
+      <c r="F19" s="60"/>
+      <c r="G19" s="60"/>
+      <c r="H19" s="60"/>
+      <c r="I19" s="61"/>
     </row>
     <row r="20" spans="1:9" ht="20.7" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="43"/>
-      <c r="B20" s="13" t="s">
+      <c r="A20" s="63"/>
+      <c r="B20" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="D20" s="19"/>
-      <c r="E20" s="12" t="s">
+      <c r="D20" s="45"/>
+      <c r="E20" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="39"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="22"/>
     </row>
     <row r="21" spans="1:9" ht="23.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="43"/>
-      <c r="B21" s="13" t="s">
+      <c r="A21" s="63"/>
+      <c r="B21" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="D21" s="19"/>
-      <c r="E21" s="12" t="s">
+      <c r="D21" s="45"/>
+      <c r="E21" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="39"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="22"/>
     </row>
     <row r="22" spans="1:9" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="43"/>
-      <c r="B22" s="13" t="s">
+      <c r="A22" s="63"/>
+      <c r="B22" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="D22" s="19"/>
-      <c r="E22" s="12" t="s">
+      <c r="D22" s="45"/>
+      <c r="E22" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="39"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="22"/>
     </row>
     <row r="23" spans="1:9" ht="38.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="43"/>
-      <c r="B23" s="13" t="s">
+      <c r="A23" s="63"/>
+      <c r="B23" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="D23" s="19"/>
-      <c r="E23" s="12" t="s">
+      <c r="D23" s="45"/>
+      <c r="E23" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="39"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="22"/>
     </row>
     <row r="24" spans="1:9" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="43"/>
-      <c r="B24" s="13" t="s">
+      <c r="A24" s="63"/>
+      <c r="B24" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="D24" s="19"/>
-      <c r="E24" s="12" t="s">
+      <c r="D24" s="45"/>
+      <c r="E24" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="39"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="22"/>
     </row>
     <row r="25" spans="1:9" ht="50.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="43"/>
-      <c r="B25" s="13" t="s">
+      <c r="A25" s="63"/>
+      <c r="B25" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="D25" s="19"/>
-      <c r="E25" s="12" t="s">
+      <c r="D25" s="45"/>
+      <c r="E25" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="39"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="22"/>
     </row>
     <row r="26" spans="1:9" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="43"/>
-      <c r="B26" s="13" t="s">
+      <c r="A26" s="63"/>
+      <c r="B26" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="C26" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="D26" s="19"/>
-      <c r="E26" s="12" t="s">
+      <c r="D26" s="45"/>
+      <c r="E26" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="39"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="22"/>
     </row>
     <row r="27" spans="1:9" ht="73.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="43"/>
-      <c r="B27" s="13" t="s">
+      <c r="A27" s="63"/>
+      <c r="B27" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="C27" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="D27" s="19"/>
-      <c r="E27" s="12" t="s">
+      <c r="D27" s="45"/>
+      <c r="E27" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="39"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="22"/>
     </row>
     <row r="28" spans="1:9" ht="33.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="43"/>
-      <c r="B28" s="13" t="s">
+      <c r="A28" s="63"/>
+      <c r="B28" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="C28" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="D28" s="19"/>
-      <c r="E28" s="12" t="s">
+      <c r="D28" s="45"/>
+      <c r="E28" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
-      <c r="H28" s="18"/>
-      <c r="I28" s="40"/>
+      <c r="F28" s="46"/>
+      <c r="G28" s="46"/>
+      <c r="H28" s="46"/>
+      <c r="I28" s="47"/>
     </row>
     <row r="29" spans="1:9" ht="57.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="44"/>
-      <c r="B29" s="14" t="s">
+      <c r="A29" s="64"/>
+      <c r="B29" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C29" s="11" t="s">
+      <c r="C29" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="D29" s="19"/>
-      <c r="E29" s="17" t="s">
+      <c r="D29" s="45"/>
+      <c r="E29" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="16"/>
-      <c r="I29" s="41"/>
+      <c r="F29" s="48"/>
+      <c r="G29" s="48"/>
+      <c r="H29" s="48"/>
+      <c r="I29" s="49"/>
     </row>
     <row r="30" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A30" s="45">
+      <c r="A30" s="29">
         <v>2</v>
       </c>
-      <c r="B30" s="60" t="s">
+      <c r="B30" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="60"/>
-      <c r="D30" s="60"/>
-      <c r="E30" s="60"/>
-      <c r="F30" s="60"/>
-      <c r="G30" s="60"/>
-      <c r="H30" s="60"/>
-      <c r="I30" s="61"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="18"/>
+      <c r="I30" s="19"/>
     </row>
     <row r="31" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="46"/>
-      <c r="B31" s="10"/>
-      <c r="C31" s="15" t="s">
+      <c r="A31" s="30"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="D31" s="12"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="12"/>
-      <c r="G31" s="12"/>
-      <c r="H31" s="12"/>
-      <c r="I31" s="39"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="21"/>
+      <c r="H31" s="21"/>
+      <c r="I31" s="22"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="46"/>
-      <c r="B32" s="10"/>
-      <c r="C32" s="20"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="9"/>
-      <c r="I32" s="38"/>
+      <c r="A32" s="30"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="23"/>
+      <c r="D32" s="24"/>
+      <c r="E32" s="24"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="24"/>
+      <c r="H32" s="24"/>
+      <c r="I32" s="25"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="46"/>
-      <c r="B33" s="10"/>
-      <c r="C33" s="20"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="9"/>
-      <c r="I33" s="38"/>
+      <c r="A33" s="30"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="23"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="24"/>
+      <c r="H33" s="24"/>
+      <c r="I33" s="25"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" s="46"/>
-      <c r="B34" s="10"/>
-      <c r="C34" s="20"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="9"/>
-      <c r="G34" s="9"/>
-      <c r="H34" s="9"/>
-      <c r="I34" s="38"/>
+      <c r="A34" s="30"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="23"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="24"/>
+      <c r="H34" s="24"/>
+      <c r="I34" s="25"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" s="46"/>
-      <c r="B35" s="10"/>
-      <c r="C35" s="20"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="9"/>
-      <c r="H35" s="9"/>
-      <c r="I35" s="38"/>
+      <c r="A35" s="30"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="23"/>
+      <c r="D35" s="24"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="24"/>
+      <c r="G35" s="24"/>
+      <c r="H35" s="24"/>
+      <c r="I35" s="25"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" s="46"/>
-      <c r="B36" s="10"/>
-      <c r="C36" s="20"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="9"/>
-      <c r="G36" s="9"/>
-      <c r="H36" s="9"/>
-      <c r="I36" s="38"/>
+      <c r="A36" s="30"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="23"/>
+      <c r="D36" s="24"/>
+      <c r="E36" s="24"/>
+      <c r="F36" s="24"/>
+      <c r="G36" s="24"/>
+      <c r="H36" s="24"/>
+      <c r="I36" s="25"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" s="46"/>
-      <c r="B37" s="22" t="s">
+      <c r="A37" s="30"/>
+      <c r="B37" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C37" s="48" t="s">
+      <c r="C37" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="D37" s="49"/>
-      <c r="E37" s="49"/>
-      <c r="F37" s="49"/>
-      <c r="G37" s="49"/>
-      <c r="H37" s="49"/>
-      <c r="I37" s="50"/>
+      <c r="D37" s="42"/>
+      <c r="E37" s="42"/>
+      <c r="F37" s="42"/>
+      <c r="G37" s="42"/>
+      <c r="H37" s="42"/>
+      <c r="I37" s="43"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" s="46"/>
-      <c r="B38" s="14"/>
-      <c r="C38" s="23" t="s">
+      <c r="A38" s="30"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="D38" s="15" t="s">
+      <c r="D38" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="E38" s="12"/>
-      <c r="F38" s="12"/>
-      <c r="G38" s="12"/>
-      <c r="H38" s="12"/>
-      <c r="I38" s="39"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="21"/>
+      <c r="H38" s="21"/>
+      <c r="I38" s="22"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" s="46"/>
-      <c r="B39" s="14"/>
-      <c r="C39" s="14"/>
-      <c r="D39" s="20"/>
-      <c r="E39" s="9"/>
-      <c r="F39" s="9"/>
-      <c r="G39" s="9"/>
-      <c r="H39" s="9"/>
-      <c r="I39" s="38"/>
+      <c r="A39" s="30"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="23"/>
+      <c r="E39" s="24"/>
+      <c r="F39" s="24"/>
+      <c r="G39" s="24"/>
+      <c r="H39" s="24"/>
+      <c r="I39" s="25"/>
     </row>
     <row r="40" spans="1:9" ht="18.3" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" s="46"/>
-      <c r="B40" s="14"/>
-      <c r="C40" s="25"/>
-      <c r="D40" s="54"/>
-      <c r="E40" s="55"/>
-      <c r="F40" s="55"/>
-      <c r="G40" s="55"/>
-      <c r="H40" s="55"/>
-      <c r="I40" s="56"/>
+      <c r="A40" s="30"/>
+      <c r="B40" s="11"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="26"/>
+      <c r="E40" s="27"/>
+      <c r="F40" s="27"/>
+      <c r="G40" s="27"/>
+      <c r="H40" s="27"/>
+      <c r="I40" s="28"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" s="46"/>
-      <c r="B41" s="14"/>
-      <c r="C41" s="23" t="s">
+      <c r="A41" s="30"/>
+      <c r="B41" s="11"/>
+      <c r="C41" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="D41" s="21" t="s">
+      <c r="D41" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="E41" s="17"/>
-      <c r="F41" s="17"/>
-      <c r="G41" s="17"/>
-      <c r="H41" s="17"/>
-      <c r="I41" s="24"/>
+      <c r="E41" s="36"/>
+      <c r="F41" s="36"/>
+      <c r="G41" s="36"/>
+      <c r="H41" s="36"/>
+      <c r="I41" s="37"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" s="47"/>
-      <c r="B42" s="25"/>
-      <c r="C42" s="25"/>
-      <c r="D42" s="26"/>
-      <c r="E42" s="27"/>
-      <c r="F42" s="27"/>
-      <c r="G42" s="27"/>
-      <c r="H42" s="27"/>
-      <c r="I42" s="28"/>
+      <c r="A42" s="31"/>
+      <c r="B42" s="14"/>
+      <c r="C42" s="14"/>
+      <c r="D42" s="38"/>
+      <c r="E42" s="39"/>
+      <c r="F42" s="39"/>
+      <c r="G42" s="39"/>
+      <c r="H42" s="39"/>
+      <c r="I42" s="40"/>
     </row>
     <row r="43" spans="1:9" ht="18.3" x14ac:dyDescent="0.7">
-      <c r="A43" s="45">
+      <c r="A43" s="29">
         <v>3</v>
       </c>
-      <c r="B43" s="59" t="s">
+      <c r="B43" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="C43" s="60"/>
-      <c r="D43" s="60"/>
-      <c r="E43" s="60"/>
-      <c r="F43" s="60"/>
-      <c r="G43" s="60"/>
-      <c r="H43" s="60"/>
-      <c r="I43" s="61"/>
+      <c r="C43" s="18"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="18"/>
+      <c r="F43" s="18"/>
+      <c r="G43" s="18"/>
+      <c r="H43" s="18"/>
+      <c r="I43" s="19"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" s="46"/>
-      <c r="B44" s="51" t="s">
+      <c r="A44" s="30"/>
+      <c r="B44" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="C44" s="52" t="s">
+      <c r="C44" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="D44" s="15" t="s">
+      <c r="D44" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="E44" s="12"/>
-      <c r="F44" s="12"/>
-      <c r="G44" s="12"/>
-      <c r="H44" s="12"/>
-      <c r="I44" s="39"/>
+      <c r="E44" s="21"/>
+      <c r="F44" s="21"/>
+      <c r="G44" s="21"/>
+      <c r="H44" s="21"/>
+      <c r="I44" s="22"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A45" s="46"/>
-      <c r="B45" s="51"/>
-      <c r="C45" s="51"/>
-      <c r="D45" s="20"/>
-      <c r="E45" s="9"/>
-      <c r="F45" s="9"/>
-      <c r="G45" s="9"/>
-      <c r="H45" s="9"/>
-      <c r="I45" s="38"/>
+      <c r="A45" s="30"/>
+      <c r="B45" s="32"/>
+      <c r="C45" s="32"/>
+      <c r="D45" s="23"/>
+      <c r="E45" s="24"/>
+      <c r="F45" s="24"/>
+      <c r="G45" s="24"/>
+      <c r="H45" s="24"/>
+      <c r="I45" s="25"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A46" s="46"/>
-      <c r="B46" s="51"/>
-      <c r="C46" s="53"/>
-      <c r="D46" s="54"/>
-      <c r="E46" s="55"/>
-      <c r="F46" s="55"/>
-      <c r="G46" s="55"/>
-      <c r="H46" s="55"/>
-      <c r="I46" s="56"/>
+      <c r="A46" s="30"/>
+      <c r="B46" s="32"/>
+      <c r="C46" s="33"/>
+      <c r="D46" s="26"/>
+      <c r="E46" s="27"/>
+      <c r="F46" s="27"/>
+      <c r="G46" s="27"/>
+      <c r="H46" s="27"/>
+      <c r="I46" s="28"/>
     </row>
     <row r="47" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A47" s="46"/>
-      <c r="B47" s="51" t="s">
+      <c r="A47" s="30"/>
+      <c r="B47" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="C47" s="52" t="s">
+      <c r="C47" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="D47" s="15" t="s">
+      <c r="D47" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="E47" s="12"/>
-      <c r="F47" s="12"/>
-      <c r="G47" s="12"/>
-      <c r="H47" s="12"/>
-      <c r="I47" s="39"/>
+      <c r="E47" s="21"/>
+      <c r="F47" s="21"/>
+      <c r="G47" s="21"/>
+      <c r="H47" s="21"/>
+      <c r="I47" s="22"/>
     </row>
     <row r="48" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A48" s="46"/>
-      <c r="B48" s="51"/>
-      <c r="C48" s="51"/>
-      <c r="D48" s="20"/>
-      <c r="E48" s="9"/>
-      <c r="F48" s="9"/>
-      <c r="G48" s="9"/>
-      <c r="H48" s="9"/>
-      <c r="I48" s="38"/>
+      <c r="A48" s="30"/>
+      <c r="B48" s="32"/>
+      <c r="C48" s="32"/>
+      <c r="D48" s="23"/>
+      <c r="E48" s="24"/>
+      <c r="F48" s="24"/>
+      <c r="G48" s="24"/>
+      <c r="H48" s="24"/>
+      <c r="I48" s="25"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A49" s="46"/>
-      <c r="B49" s="51"/>
-      <c r="C49" s="53"/>
-      <c r="D49" s="54"/>
-      <c r="E49" s="55"/>
-      <c r="F49" s="55"/>
-      <c r="G49" s="55"/>
-      <c r="H49" s="55"/>
-      <c r="I49" s="56"/>
+      <c r="A49" s="30"/>
+      <c r="B49" s="32"/>
+      <c r="C49" s="33"/>
+      <c r="D49" s="26"/>
+      <c r="E49" s="27"/>
+      <c r="F49" s="27"/>
+      <c r="G49" s="27"/>
+      <c r="H49" s="27"/>
+      <c r="I49" s="28"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A50" s="46"/>
-      <c r="B50" s="51" t="s">
+      <c r="A50" s="30"/>
+      <c r="B50" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="C50" s="51" t="s">
+      <c r="C50" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="D50" s="15" t="s">
+      <c r="D50" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="E50" s="12"/>
-      <c r="F50" s="12"/>
-      <c r="G50" s="12"/>
-      <c r="H50" s="12"/>
-      <c r="I50" s="39"/>
+      <c r="E50" s="21"/>
+      <c r="F50" s="21"/>
+      <c r="G50" s="21"/>
+      <c r="H50" s="21"/>
+      <c r="I50" s="22"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A51" s="46"/>
-      <c r="B51" s="51"/>
-      <c r="C51" s="51"/>
-      <c r="D51" s="20"/>
-      <c r="E51" s="9"/>
-      <c r="F51" s="9"/>
-      <c r="G51" s="9"/>
-      <c r="H51" s="9"/>
-      <c r="I51" s="38"/>
+      <c r="A51" s="30"/>
+      <c r="B51" s="32"/>
+      <c r="C51" s="32"/>
+      <c r="D51" s="23"/>
+      <c r="E51" s="24"/>
+      <c r="F51" s="24"/>
+      <c r="G51" s="24"/>
+      <c r="H51" s="24"/>
+      <c r="I51" s="25"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A52" s="47"/>
-      <c r="B52" s="53"/>
-      <c r="C52" s="53"/>
-      <c r="D52" s="54"/>
-      <c r="E52" s="55"/>
-      <c r="F52" s="55"/>
-      <c r="G52" s="55"/>
-      <c r="H52" s="55"/>
-      <c r="I52" s="56"/>
+      <c r="A52" s="31"/>
+      <c r="B52" s="33"/>
+      <c r="C52" s="33"/>
+      <c r="D52" s="26"/>
+      <c r="E52" s="27"/>
+      <c r="F52" s="27"/>
+      <c r="G52" s="27"/>
+      <c r="H52" s="27"/>
+      <c r="I52" s="28"/>
     </row>
     <row r="53" spans="1:9" ht="18.3" x14ac:dyDescent="0.7">
-      <c r="A53" s="45">
+      <c r="A53" s="29">
         <v>4</v>
       </c>
-      <c r="B53" s="59" t="s">
+      <c r="B53" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="C53" s="60"/>
-      <c r="D53" s="60"/>
-      <c r="E53" s="60"/>
-      <c r="F53" s="60"/>
-      <c r="G53" s="60"/>
-      <c r="H53" s="60"/>
-      <c r="I53" s="61"/>
+      <c r="C53" s="18"/>
+      <c r="D53" s="18"/>
+      <c r="E53" s="18"/>
+      <c r="F53" s="18"/>
+      <c r="G53" s="18"/>
+      <c r="H53" s="18"/>
+      <c r="I53" s="19"/>
     </row>
     <row r="54" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A54" s="46"/>
-      <c r="B54" s="46" t="s">
+      <c r="A54" s="30"/>
+      <c r="B54" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="C54" s="15" t="s">
+      <c r="C54" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="D54" s="12"/>
-      <c r="E54" s="12"/>
-      <c r="F54" s="12"/>
-      <c r="G54" s="12"/>
-      <c r="H54" s="12"/>
-      <c r="I54" s="39"/>
+      <c r="D54" s="21"/>
+      <c r="E54" s="21"/>
+      <c r="F54" s="21"/>
+      <c r="G54" s="21"/>
+      <c r="H54" s="21"/>
+      <c r="I54" s="22"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A55" s="46"/>
-      <c r="B55" s="46"/>
-      <c r="C55" s="20"/>
-      <c r="D55" s="9"/>
-      <c r="E55" s="9"/>
-      <c r="F55" s="9"/>
-      <c r="G55" s="9"/>
-      <c r="H55" s="9"/>
-      <c r="I55" s="38"/>
+      <c r="A55" s="30"/>
+      <c r="B55" s="30"/>
+      <c r="C55" s="23"/>
+      <c r="D55" s="24"/>
+      <c r="E55" s="24"/>
+      <c r="F55" s="24"/>
+      <c r="G55" s="24"/>
+      <c r="H55" s="24"/>
+      <c r="I55" s="25"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A56" s="46"/>
-      <c r="B56" s="46"/>
-      <c r="C56" s="20"/>
-      <c r="D56" s="9"/>
-      <c r="E56" s="9"/>
-      <c r="F56" s="9"/>
-      <c r="G56" s="9"/>
-      <c r="H56" s="9"/>
-      <c r="I56" s="38"/>
+      <c r="A56" s="30"/>
+      <c r="B56" s="30"/>
+      <c r="C56" s="23"/>
+      <c r="D56" s="24"/>
+      <c r="E56" s="24"/>
+      <c r="F56" s="24"/>
+      <c r="G56" s="24"/>
+      <c r="H56" s="24"/>
+      <c r="I56" s="25"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A57" s="46"/>
-      <c r="B57" s="46"/>
-      <c r="C57" s="20"/>
-      <c r="D57" s="9"/>
-      <c r="E57" s="9"/>
-      <c r="F57" s="9"/>
-      <c r="G57" s="9"/>
-      <c r="H57" s="9"/>
-      <c r="I57" s="38"/>
+      <c r="A57" s="30"/>
+      <c r="B57" s="30"/>
+      <c r="C57" s="23"/>
+      <c r="D57" s="24"/>
+      <c r="E57" s="24"/>
+      <c r="F57" s="24"/>
+      <c r="G57" s="24"/>
+      <c r="H57" s="24"/>
+      <c r="I57" s="25"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A58" s="46"/>
-      <c r="B58" s="46"/>
-      <c r="C58" s="20"/>
-      <c r="D58" s="9"/>
-      <c r="E58" s="9"/>
-      <c r="F58" s="9"/>
-      <c r="G58" s="9"/>
-      <c r="H58" s="9"/>
-      <c r="I58" s="38"/>
+      <c r="A58" s="30"/>
+      <c r="B58" s="30"/>
+      <c r="C58" s="23"/>
+      <c r="D58" s="24"/>
+      <c r="E58" s="24"/>
+      <c r="F58" s="24"/>
+      <c r="G58" s="24"/>
+      <c r="H58" s="24"/>
+      <c r="I58" s="25"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A59" s="46"/>
-      <c r="B59" s="46"/>
-      <c r="C59" s="20"/>
-      <c r="D59" s="9"/>
-      <c r="E59" s="9"/>
-      <c r="F59" s="9"/>
-      <c r="G59" s="9"/>
-      <c r="H59" s="9"/>
-      <c r="I59" s="38"/>
+      <c r="A59" s="30"/>
+      <c r="B59" s="30"/>
+      <c r="C59" s="23"/>
+      <c r="D59" s="24"/>
+      <c r="E59" s="24"/>
+      <c r="F59" s="24"/>
+      <c r="G59" s="24"/>
+      <c r="H59" s="24"/>
+      <c r="I59" s="25"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A60" s="46"/>
-      <c r="B60" s="46"/>
-      <c r="C60" s="20"/>
-      <c r="D60" s="9"/>
-      <c r="E60" s="9"/>
-      <c r="F60" s="9"/>
-      <c r="G60" s="9"/>
-      <c r="H60" s="9"/>
-      <c r="I60" s="38"/>
+      <c r="A60" s="30"/>
+      <c r="B60" s="30"/>
+      <c r="C60" s="23"/>
+      <c r="D60" s="24"/>
+      <c r="E60" s="24"/>
+      <c r="F60" s="24"/>
+      <c r="G60" s="24"/>
+      <c r="H60" s="24"/>
+      <c r="I60" s="25"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A61" s="46"/>
-      <c r="B61" s="46"/>
-      <c r="C61" s="20"/>
-      <c r="D61" s="9"/>
-      <c r="E61" s="9"/>
-      <c r="F61" s="9"/>
-      <c r="G61" s="9"/>
-      <c r="H61" s="9"/>
-      <c r="I61" s="38"/>
+      <c r="A61" s="30"/>
+      <c r="B61" s="30"/>
+      <c r="C61" s="23"/>
+      <c r="D61" s="24"/>
+      <c r="E61" s="24"/>
+      <c r="F61" s="24"/>
+      <c r="G61" s="24"/>
+      <c r="H61" s="24"/>
+      <c r="I61" s="25"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A62" s="46"/>
-      <c r="B62" s="46"/>
-      <c r="C62" s="20"/>
-      <c r="D62" s="9"/>
-      <c r="E62" s="9"/>
-      <c r="F62" s="9"/>
-      <c r="G62" s="9"/>
-      <c r="H62" s="9"/>
-      <c r="I62" s="38"/>
+      <c r="A62" s="30"/>
+      <c r="B62" s="30"/>
+      <c r="C62" s="23"/>
+      <c r="D62" s="24"/>
+      <c r="E62" s="24"/>
+      <c r="F62" s="24"/>
+      <c r="G62" s="24"/>
+      <c r="H62" s="24"/>
+      <c r="I62" s="25"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A63" s="47"/>
-      <c r="B63" s="47"/>
-      <c r="C63" s="54"/>
-      <c r="D63" s="55"/>
-      <c r="E63" s="55"/>
-      <c r="F63" s="55"/>
-      <c r="G63" s="55"/>
-      <c r="H63" s="55"/>
-      <c r="I63" s="56"/>
+      <c r="A63" s="31"/>
+      <c r="B63" s="31"/>
+      <c r="C63" s="26"/>
+      <c r="D63" s="27"/>
+      <c r="E63" s="27"/>
+      <c r="F63" s="27"/>
+      <c r="G63" s="27"/>
+      <c r="H63" s="27"/>
+      <c r="I63" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="B53:I53"/>
-    <mergeCell ref="C54:I63"/>
-    <mergeCell ref="A53:A63"/>
-    <mergeCell ref="B54:B63"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="B50:B52"/>
-    <mergeCell ref="A43:A52"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="A19:A29"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I9"/>
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="A11:I18"/>
+    <mergeCell ref="B19:I19"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E20:I20"/>
+    <mergeCell ref="E21:I21"/>
+    <mergeCell ref="E22:I22"/>
+    <mergeCell ref="E23:I23"/>
+    <mergeCell ref="E24:I24"/>
+    <mergeCell ref="E25:I25"/>
+    <mergeCell ref="E26:I26"/>
+    <mergeCell ref="E27:I27"/>
+    <mergeCell ref="E28:I28"/>
+    <mergeCell ref="E29:I29"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
     <mergeCell ref="A30:A42"/>
     <mergeCell ref="B43:I43"/>
     <mergeCell ref="D47:I49"/>
@@ -2235,32 +2253,14 @@
     <mergeCell ref="D44:I46"/>
     <mergeCell ref="B30:I30"/>
     <mergeCell ref="C37:I37"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="E20:I20"/>
-    <mergeCell ref="E21:I21"/>
-    <mergeCell ref="E22:I22"/>
-    <mergeCell ref="E23:I23"/>
-    <mergeCell ref="E24:I24"/>
-    <mergeCell ref="E25:I25"/>
-    <mergeCell ref="E26:I26"/>
-    <mergeCell ref="E27:I27"/>
-    <mergeCell ref="E28:I28"/>
-    <mergeCell ref="E29:I29"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:I9"/>
-    <mergeCell ref="A10:I10"/>
-    <mergeCell ref="A11:I18"/>
-    <mergeCell ref="B19:I19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="A19:A29"/>
+    <mergeCell ref="B53:I53"/>
+    <mergeCell ref="C54:I63"/>
+    <mergeCell ref="A53:A63"/>
+    <mergeCell ref="B54:B63"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="B50:B52"/>
+    <mergeCell ref="A43:A52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -2323,10 +2323,10 @@
     </row>
     <row r="2" spans="1:10" ht="216" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="B2" s="57" t="s">
-        <v>177</v>
+        <v>174</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>175</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>10</v>
@@ -2347,10 +2347,10 @@
         <v>94</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -2462,7 +2462,7 @@
         <v>90</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="I9" s="6"/>
       <c r="J9" s="8"/>
@@ -2475,10 +2475,10 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="I10" s="6"/>
       <c r="J10" s="8"/>
@@ -2579,10 +2579,10 @@
     </row>
     <row r="2" spans="1:10" ht="239.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="B2" s="57" t="s">
-        <v>183</v>
+        <v>180</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>181</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>10</v>
@@ -2591,7 +2591,7 @@
         <v>11</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>13</v>
@@ -2718,7 +2718,7 @@
         <v>90</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="I9" s="6"/>
       <c r="J9" s="8"/>
@@ -2731,10 +2731,10 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="I10" s="6"/>
       <c r="J10" s="8"/>
@@ -2747,10 +2747,10 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I11" s="6"/>
       <c r="J11" s="8"/>
@@ -2788,8 +2788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="77" workbookViewId="0">
-      <selection sqref="A1:J13"/>
+    <sheetView zoomScale="77" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3002,7 +3002,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EBA8D0F-FA1A-48F3-B60B-00BC5DF66123}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -3056,7 +3056,7 @@
       <c r="A2" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B2" s="57" t="s">
+      <c r="B2" s="15" t="s">
         <v>73</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -3065,8 +3065,8 @@
       <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="57" t="s">
-        <v>132</v>
+      <c r="E2" s="15" t="s">
+        <v>130</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>13</v>
@@ -3142,7 +3142,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>81</v>
@@ -3301,7 +3301,7 @@
       <c r="A2" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B2" s="57" t="s">
+      <c r="B2" s="15" t="s">
         <v>93</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -3310,8 +3310,8 @@
       <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="57" t="s">
-        <v>133</v>
+      <c r="E2" s="15" t="s">
+        <v>131</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>13</v>
@@ -3566,7 +3566,7 @@
       <c r="A2" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B2" s="57" t="s">
+      <c r="B2" s="15" t="s">
         <v>106</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -3576,7 +3576,7 @@
         <v>11</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>13</v>
@@ -3710,7 +3710,7 @@
       <c r="I9" s="6"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:10" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -3771,8 +3771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FACE536-9F56-44F1-B9C1-D7AFBBB4D88C}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView topLeftCell="C9" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:H17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3825,8 +3825,8 @@
       <c r="A2" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B2" s="57" t="s">
-        <v>118</v>
+      <c r="B2" s="15" t="s">
+        <v>187</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>10</v>
@@ -3835,7 +3835,7 @@
         <v>11</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>119</v>
+        <v>186</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>13</v>
@@ -3912,7 +3912,7 @@
         <v>109</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="I6" s="6"/>
       <c r="J6" s="8"/>
@@ -3928,7 +3928,7 @@
         <v>110</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="I7" s="6"/>
       <c r="J7" s="8"/>
@@ -3944,7 +3944,7 @@
         <v>111</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="I8" s="6"/>
       <c r="J8" s="8"/>
@@ -3960,7 +3960,7 @@
         <v>91</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="I9" s="6"/>
       <c r="J9" s="8"/>
@@ -3976,7 +3976,7 @@
         <v>92</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="I10" s="6"/>
       <c r="J10" s="8"/>
@@ -3989,10 +3989,10 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="I11" s="6"/>
       <c r="J11" s="8"/>
@@ -4005,10 +4005,10 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I12" s="6"/>
       <c r="J12" s="8"/>
@@ -4021,44 +4021,44 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I13" s="6"/>
       <c r="J13" s="8"/>
     </row>
     <row r="14" spans="1:10" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="G14" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="G15" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="H15" s="58" t="s">
-        <v>129</v>
+        <v>122</v>
+      </c>
+      <c r="H15" s="16" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="G16" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="H16" s="58" t="s">
-        <v>130</v>
+        <v>123</v>
+      </c>
+      <c r="H16" s="16" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="17" spans="7:8" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="G17" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="H17" s="58" t="s">
-        <v>131</v>
+        <v>124</v>
+      </c>
+      <c r="H17" s="16" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -4070,8 +4070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B6B8225-13D8-4953-92D6-8112B577B21E}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView topLeftCell="C8" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:H12"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -4122,10 +4122,10 @@
     </row>
     <row r="2" spans="1:10" ht="155.1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="B2" s="57" t="s">
-        <v>143</v>
+        <v>140</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>141</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>10</v>
@@ -4134,7 +4134,7 @@
         <v>11</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>13</v>
@@ -4261,7 +4261,7 @@
         <v>90</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="I9" s="6"/>
       <c r="J9" s="8"/>
@@ -4293,7 +4293,7 @@
         <v>92</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="I11" s="6"/>
       <c r="J11" s="8"/>
@@ -4306,10 +4306,10 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="I12" s="6"/>
       <c r="J12" s="8"/>
@@ -4387,10 +4387,10 @@
     </row>
     <row r="2" spans="1:10" ht="188.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="B2" s="57" t="s">
-        <v>150</v>
+        <v>147</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>148</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>10</v>
@@ -4399,7 +4399,7 @@
         <v>11</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>13</v>
@@ -4411,10 +4411,10 @@
         <v>79</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -4480,7 +4480,7 @@
         <v>109</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="I6" s="6"/>
       <c r="J6" s="8"/>
@@ -4496,7 +4496,7 @@
         <v>110</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="I7" s="6"/>
       <c r="J7" s="8"/>
@@ -4512,7 +4512,7 @@
         <v>111</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="I8" s="6"/>
       <c r="J8" s="8"/>
@@ -4528,7 +4528,7 @@
         <v>91</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="I9" s="6"/>
       <c r="J9" s="8"/>
@@ -4544,7 +4544,7 @@
         <v>92</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="I10" s="6"/>
       <c r="J10" s="8"/>
@@ -4557,10 +4557,10 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I11" s="6"/>
       <c r="J11" s="8"/>
@@ -4573,10 +4573,10 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="I12" s="6"/>
       <c r="J12" s="8"/>
@@ -4589,33 +4589,33 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="I13" s="6"/>
       <c r="J13" s="8"/>
     </row>
     <row r="14" spans="1:10" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="G14" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="G15" s="2"/>
-      <c r="H15" s="58"/>
+      <c r="H15" s="16"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="G16" s="2"/>
-      <c r="H16" s="58"/>
+      <c r="H16" s="16"/>
     </row>
     <row r="17" spans="7:8" x14ac:dyDescent="0.55000000000000004">
       <c r="G17" s="2"/>
-      <c r="H17" s="58"/>
+      <c r="H17" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4678,10 +4678,10 @@
     </row>
     <row r="2" spans="1:10" ht="221.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="B2" s="57" t="s">
-        <v>163</v>
+        <v>160</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>161</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>10</v>
@@ -4689,8 +4689,8 @@
       <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="57" t="s">
-        <v>164</v>
+      <c r="E2" s="15" t="s">
+        <v>162</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>13</v>
@@ -4702,10 +4702,10 @@
         <v>79</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -4771,7 +4771,7 @@
         <v>109</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="I6" s="6"/>
       <c r="J6" s="8"/>
@@ -4787,7 +4787,7 @@
         <v>110</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="I7" s="6"/>
       <c r="J7" s="8"/>
@@ -4803,7 +4803,7 @@
         <v>111</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="I8" s="6"/>
       <c r="J8" s="8"/>
@@ -4816,10 +4816,10 @@
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="I9" s="6"/>
       <c r="J9" s="8"/>
@@ -4832,10 +4832,10 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="I10" s="6"/>
       <c r="J10" s="8"/>
@@ -4848,15 +4848,15 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="I11" s="6"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -4864,10 +4864,10 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="H12" s="2" t="s">
         <v>170</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>172</v>
       </c>
       <c r="I12" s="6"/>
       <c r="J12" s="8"/>
@@ -4880,10 +4880,10 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>173</v>
       </c>
       <c r="I13" s="6"/>
       <c r="J13" s="8"/>

</xml_diff>